<commit_message>
chore: Actualizar rutas de la aplicación Preoperacional_app
</commit_message>
<xml_diff>
--- a/Pruebas_excel/02. HOJAS DE VIDA VEHICULOS/KWO 032/Hoja de vida/KWO 032.xlsx
+++ b/Pruebas_excel/02. HOJAS DE VIDA VEHICULOS/KWO 032/Hoja de vida/KWO 032.xlsx
@@ -1594,10 +1594,8 @@
         </is>
       </c>
       <c r="H11" s="107" t="n"/>
-      <c r="I11" s="47" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
+      <c r="I11" s="47" t="n">
+        <v>45524</v>
       </c>
       <c r="J11" s="112" t="n"/>
       <c r="K11" s="107" t="n"/>
@@ -1636,10 +1634,8 @@
         </is>
       </c>
       <c r="H12" s="117" t="n"/>
-      <c r="I12" s="47" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
+      <c r="I12" s="47" t="n">
+        <v>45524</v>
       </c>
       <c r="J12" s="116" t="n"/>
       <c r="K12" s="117" t="n"/>
@@ -1675,7 +1671,7 @@
       <c r="N13" s="112" t="n"/>
       <c r="O13" s="107" t="n"/>
       <c r="P13" s="3" t="n">
-        <v>100220540</v>
+        <v>200125</v>
       </c>
     </row>
     <row r="14" ht="18" customHeight="1">
@@ -1698,10 +1694,8 @@
       <c r="M14" s="112" t="n"/>
       <c r="N14" s="112" t="n"/>
       <c r="O14" s="107" t="n"/>
-      <c r="P14" s="4" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
+      <c r="P14" s="4" t="n">
+        <v>45524</v>
       </c>
     </row>
     <row r="15" ht="3" customHeight="1">

</xml_diff>

<commit_message>
Agrgando Mtto_equipos_de_computo & Pre_Op_equipos_medicion_app al proyecto y modificacion a la app Preoperacional_app de correccion de errores y adicion funcionalidades.
</commit_message>
<xml_diff>
--- a/Pruebas_excel/02. HOJAS DE VIDA VEHICULOS/KWO 032/Hoja de vida/KWO 032.xlsx
+++ b/Pruebas_excel/02. HOJAS DE VIDA VEHICULOS/KWO 032/Hoja de vida/KWO 032.xlsx
@@ -1364,7 +1364,7 @@
       <c r="F5" s="107" t="n"/>
       <c r="G5" s="22" t="inlineStr">
         <is>
-          <t>Suzuki</t>
+          <t>SUZUKI</t>
         </is>
       </c>
       <c r="H5" s="107" t="n"/>
@@ -1541,7 +1541,7 @@
       <c r="C10" s="107" t="n"/>
       <c r="D10" s="43" t="inlineStr">
         <is>
-          <t>10017861890</t>
+          <t>10024856311</t>
         </is>
       </c>
       <c r="E10" s="112" t="n"/>
@@ -1554,7 +1554,7 @@
       <c r="H10" s="107" t="n"/>
       <c r="I10" s="43" t="inlineStr">
         <is>
-          <t>1000115505001</t>
+          <t>SEGUROS MUNDIAL</t>
         </is>
       </c>
       <c r="J10" s="112" t="n"/>
@@ -1583,7 +1583,7 @@
       <c r="C11" s="107" t="n"/>
       <c r="D11" s="46" t="inlineStr">
         <is>
-          <t>BOGOTA</t>
+          <t>352021000457021</t>
         </is>
       </c>
       <c r="E11" s="112" t="n"/>
@@ -1595,7 +1595,7 @@
       </c>
       <c r="H11" s="107" t="n"/>
       <c r="I11" s="47" t="n">
-        <v>45524</v>
+        <v>45279</v>
       </c>
       <c r="J11" s="112" t="n"/>
       <c r="K11" s="107" t="n"/>
@@ -1634,8 +1634,10 @@
         </is>
       </c>
       <c r="H12" s="117" t="n"/>
-      <c r="I12" s="47" t="n">
-        <v>45524</v>
+      <c r="I12" s="47" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
       </c>
       <c r="J12" s="116" t="n"/>
       <c r="K12" s="117" t="n"/>
@@ -1649,7 +1651,7 @@
       <c r="O12" s="107" t="n"/>
       <c r="P12" s="2" t="inlineStr">
         <is>
-          <t>DEL ESTADO</t>
+          <t>LIBERTY SEGUROS</t>
         </is>
       </c>
     </row>
@@ -1671,7 +1673,7 @@
       <c r="N13" s="112" t="n"/>
       <c r="O13" s="107" t="n"/>
       <c r="P13" s="3" t="n">
-        <v>200125</v>
+        <v>522044</v>
       </c>
     </row>
     <row r="14" ht="18" customHeight="1">
@@ -1695,7 +1697,7 @@
       <c r="N14" s="112" t="n"/>
       <c r="O14" s="107" t="n"/>
       <c r="P14" s="4" t="n">
-        <v>45524</v>
+        <v>45566</v>
       </c>
     </row>
     <row r="15" ht="3" customHeight="1">
@@ -1792,7 +1794,7 @@
       <c r="I18" s="112" t="n"/>
       <c r="J18" s="107" t="n"/>
       <c r="K18" s="73" t="n">
-        <v>2000</v>
+        <v>998</v>
       </c>
       <c r="L18" s="112" t="n"/>
       <c r="M18" s="107" t="n"/>
@@ -1833,7 +1835,7 @@
       <c r="J19" s="107" t="n"/>
       <c r="K19" s="73" t="inlineStr">
         <is>
-          <t>4X2</t>
+          <t>4x2</t>
         </is>
       </c>
       <c r="L19" s="112" t="n"/>
@@ -1846,7 +1848,7 @@
       <c r="O19" s="107" t="n"/>
       <c r="P19" s="73" t="inlineStr">
         <is>
-          <t>5PSJPSJ</t>
+          <t>5PSjPSJ</t>
         </is>
       </c>
     </row>
@@ -1938,7 +1940,7 @@
       <c r="M22" s="107" t="n"/>
       <c r="N22" s="73" t="inlineStr">
         <is>
-          <t>Si</t>
+          <t>No</t>
         </is>
       </c>
       <c r="O22" s="112" t="n"/>
@@ -1972,7 +1974,7 @@
       <c r="M23" s="107" t="n"/>
       <c r="N23" s="73" t="inlineStr">
         <is>
-          <t>Si</t>
+          <t>No</t>
         </is>
       </c>
       <c r="O23" s="112" t="n"/>
@@ -2022,7 +2024,7 @@
       <c r="C25" s="107" t="n"/>
       <c r="D25" s="73" t="inlineStr">
         <is>
-          <t>Si</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E25" s="112" t="n"/>
@@ -2056,7 +2058,7 @@
       <c r="C26" s="107" t="n"/>
       <c r="D26" s="73" t="inlineStr">
         <is>
-          <t>Si</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E26" s="112" t="n"/>
@@ -2127,97 +2129,97 @@
     </row>
   </sheetData>
   <mergeCells count="91">
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="A17:P17"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="I12:K14"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="F1:L3"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="A9:P9"/>
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="D25:I25"/>
     <mergeCell ref="I10:K10"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="L12:O12"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="L14:O14"/>
+    <mergeCell ref="D22:I22"/>
     <mergeCell ref="J20:P20"/>
+    <mergeCell ref="A28:P31"/>
+    <mergeCell ref="D21:I21"/>
+    <mergeCell ref="M8:P8"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="G12:H14"/>
+    <mergeCell ref="J23:M23"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="A16:H16"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="A12:C14"/>
+    <mergeCell ref="I6:L6"/>
+    <mergeCell ref="K18:M18"/>
+    <mergeCell ref="I7:L7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="N22:P22"/>
+    <mergeCell ref="M7:P7"/>
+    <mergeCell ref="N21:P21"/>
+    <mergeCell ref="A25:C25"/>
     <mergeCell ref="J22:M22"/>
-    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="N23:P23"/>
+    <mergeCell ref="A18:B19"/>
+    <mergeCell ref="A4:P4"/>
+    <mergeCell ref="J21:M21"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="I16:P16"/>
     <mergeCell ref="N18:O18"/>
+    <mergeCell ref="M5:P5"/>
+    <mergeCell ref="D24:I24"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="H18:J18"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="N19:O19"/>
+    <mergeCell ref="J24:M24"/>
+    <mergeCell ref="D26:I26"/>
+    <mergeCell ref="N25:P25"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="J26:M26"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="L10:O10"/>
+    <mergeCell ref="J25:M25"/>
+    <mergeCell ref="I8:L8"/>
+    <mergeCell ref="A1:E3"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="L11:O11"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="D12:F14"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="A20:I20"/>
     <mergeCell ref="A10:C10"/>
-    <mergeCell ref="M8:P8"/>
-    <mergeCell ref="J26:M26"/>
-    <mergeCell ref="A17:P17"/>
-    <mergeCell ref="C6:D6"/>
     <mergeCell ref="K19:M19"/>
-    <mergeCell ref="D12:F14"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="A18:B19"/>
-    <mergeCell ref="M5:P5"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="M7:P7"/>
+    <mergeCell ref="N24:P24"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="L13:O13"/>
+    <mergeCell ref="D23:I23"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="N26:P26"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A27:P27"/>
+    <mergeCell ref="M6:P6"/>
     <mergeCell ref="I5:L5"/>
-    <mergeCell ref="N25:P25"/>
-    <mergeCell ref="L13:O13"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="G12:H14"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="A27:P27"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="A20:I20"/>
-    <mergeCell ref="I11:K11"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="D26:I26"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="L10:O10"/>
-    <mergeCell ref="A16:H16"/>
-    <mergeCell ref="L11:O11"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A28:P31"/>
-    <mergeCell ref="M6:P6"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="I7:L7"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="D24:I24"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="N26:P26"/>
-    <mergeCell ref="L14:O14"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="J25:M25"/>
-    <mergeCell ref="L12:O12"/>
-    <mergeCell ref="A9:P9"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="I8:L8"/>
-    <mergeCell ref="J23:M23"/>
-    <mergeCell ref="N21:P21"/>
-    <mergeCell ref="D21:I21"/>
-    <mergeCell ref="F1:L3"/>
-    <mergeCell ref="D23:I23"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="J21:M21"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="K18:M18"/>
-    <mergeCell ref="H18:J18"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="N19:O19"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A4:P4"/>
-    <mergeCell ref="D22:I22"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="N23:P23"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="D25:I25"/>
-    <mergeCell ref="A12:C14"/>
-    <mergeCell ref="A1:E3"/>
-    <mergeCell ref="J24:M24"/>
-    <mergeCell ref="N24:P24"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="I16:P16"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="N22:P22"/>
-    <mergeCell ref="O1:P1"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="I12:K14"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="I6:L6"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="O2:P2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>